<commit_message>
Proyecto medio Turnos de Riego3
</commit_message>
<xml_diff>
--- a/data/turnos_2026.xlsx
+++ b/data/turnos_2026.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\proyectos\turnos_riego\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\proyectos\turnos_riego\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E93E6859-02AE-4E63-8CE6-AABC3E5CB793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E5A952-6B11-496B-8448-0948F018E8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82EA9E55-AC67-47C7-AB88-E36128228591}"/>
   </bookViews>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="10">
-  <si>
-    <t>TURNOS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="9">
   <si>
     <t>FECHA</t>
   </si>
@@ -75,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,27 +88,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -126,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -138,15 +121,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -218,47 +192,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CADA34-1198-4F17-B262-EB7D0998CFC1}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,630 +581,615 @@
     <col min="7" max="7" width="3.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="2">
-        <v>2026</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7">
+        <v>46026</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>46034</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>46026</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="13">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>46034</v>
+      <c r="F3" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>46040</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="13">
-        <v>2</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>46040</v>
+      <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>46047</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="15">
-        <v>3</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>46047</v>
+      <c r="A6" s="7">
+        <v>46055</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>46055</v>
+      <c r="A7" s="7">
+        <v>46061</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>4</v>
+      <c r="C7" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>46061</v>
+      <c r="A8" s="7">
+        <v>46068</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>46068</v>
+      <c r="A9" s="7">
+        <v>46076</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>46076</v>
+      <c r="A10" s="7">
+        <v>46082</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>9</v>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>46082</v>
+      <c r="A11" s="7">
+        <v>46089</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>46089</v>
+      <c r="A12" s="7">
+        <v>46097</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>46097</v>
+      <c r="A13" s="7">
+        <v>46103</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>4</v>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>46103</v>
+      <c r="A14" s="7">
+        <v>46110</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>46110</v>
+      <c r="A15" s="7">
+        <v>46118</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>46118</v>
+      <c r="A16" s="7">
+        <v>46124</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>6</v>
+      <c r="C16" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>46124</v>
+      <c r="A17" s="7">
+        <v>46131</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>46131</v>
+      <c r="A18" s="7">
+        <v>46139</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>46139</v>
+      <c r="A19" s="7">
+        <v>46145</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>4</v>
+      <c r="C19" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>46145</v>
+      <c r="A20" s="7">
+        <v>46152</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>46152</v>
+      <c r="A21" s="7">
+        <v>46160</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>46160</v>
+      <c r="A22" s="7">
+        <v>46166</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>9</v>
+      <c r="C22" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
-        <v>46166</v>
+      <c r="A23" s="7">
+        <v>46173</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>46173</v>
+      <c r="A24" s="7">
+        <v>46181</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>46181</v>
+      <c r="A25" s="7">
+        <v>46187</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>4</v>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>46187</v>
+      <c r="A26" s="7">
+        <v>46194</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
-        <v>46194</v>
+      <c r="A27" s="7">
+        <v>46202</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
-        <v>46202</v>
+      <c r="A28" s="7">
+        <v>46208</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>6</v>
+      <c r="C28" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
-        <v>46208</v>
+      <c r="A29" s="7">
+        <v>46215</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
-        <v>46215</v>
+      <c r="A30" s="7">
+        <v>46223</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
-        <v>46223</v>
+      <c r="A31" s="7">
+        <v>46229</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>4</v>
+      <c r="C31" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
-        <v>46229</v>
+      <c r="A32" s="7">
+        <v>46236</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
-        <v>46236</v>
+      <c r="A33" s="7">
+        <v>46244</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
-        <v>46244</v>
+      <c r="A34" s="7">
+        <v>46250</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>9</v>
+      <c r="C34" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
-        <v>46250</v>
+      <c r="A35" s="7">
+        <v>46257</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
-        <v>46257</v>
+      <c r="A36" s="7">
+        <v>46265</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
-        <v>46265</v>
+      <c r="A37" s="7">
+        <v>46271</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>4</v>
+      <c r="C37" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
-        <v>46271</v>
+      <c r="A38" s="7">
+        <v>46278</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
-        <v>46278</v>
+      <c r="A39" s="7">
+        <v>46286</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
-        <v>46286</v>
+      <c r="A40" s="7">
+        <v>46292</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>6</v>
+      <c r="C40" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
-        <v>46292</v>
+      <c r="A41" s="7">
+        <v>46299</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
-        <v>46299</v>
+      <c r="A42" s="7">
+        <v>46307</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="11">
-        <v>46307</v>
+      <c r="A43" s="7">
+        <v>46313</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>4</v>
+      <c r="C43" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
-        <v>46313</v>
+      <c r="A44" s="7">
+        <v>46320</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
-        <v>46320</v>
+      <c r="A45" s="7">
+        <v>46328</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
-        <v>46328</v>
+      <c r="A46" s="7">
+        <v>46334</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>9</v>
+      <c r="C46" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
-        <v>46334</v>
+      <c r="A47" s="7">
+        <v>46341</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
-        <v>46341</v>
+      <c r="A48" s="7">
+        <v>46349</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
-        <v>46349</v>
+      <c r="A49" s="7">
+        <v>46355</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>4</v>
+      <c r="C49" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
-        <v>46355</v>
+      <c r="A50" s="7">
+        <v>46362</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
-        <v>46362</v>
+      <c r="A51" s="7">
+        <v>46370</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
-        <v>46370</v>
+      <c r="A52" s="7">
+        <v>46376</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
-        <v>46376</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17">
+      <c r="C52" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="13">
         <v>46383</v>
       </c>
-      <c r="B54" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>9</v>
+      <c r="B53" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A3:C54">
+  <conditionalFormatting sqref="A2:C53">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR(MOD(#REF!,4)=0,MOD(#REF!,4)=1,MOD(#REF!,4)=2)</formula>
     </cfRule>

</xml_diff>